<commit_message>
Added new implementations for LSTM and XGBoost
</commit_message>
<xml_diff>
--- a/data/BEV_vehicles/storage/BEV_vehicles_per_month.xlsx
+++ b/data/BEV_vehicles/storage/BEV_vehicles_per_month.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skyfano/Documents/Masterarbeit/Prediction_of_energy_prices/data/BEV_vehicles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skyfano/Documents/Masterarbeit/Prediction_of_energy_prices/data/BEV_vehicles/storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D36356-689E-6943-AD60-587046704985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52E89D7-4005-A440-9170-21E538E94FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="31500" xr2:uid="{FA9BD294-7823-FC4B-AB3C-054BED597FCE}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{FA9BD294-7823-FC4B-AB3C-054BED597FCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBBEB8F-BD83-764D-BDAF-EF382170D168}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,7 +735,7 @@
         <v>29740</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>29668</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -787,7 +788,7 @@
         <v>42780</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>29708</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -840,7 +841,7 @@
         <v>52988</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>43412</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -892,8 +893,8 @@
       <c r="P8">
         <v>48682</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
+      <c r="Q8" s="2">
+        <v>30762</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1227,7 +1228,7 @@
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
-        <v>81337</v>
+        <v>214887</v>
       </c>
     </row>
     <row r="24" spans="2:17" ht="22" x14ac:dyDescent="0.3">

</xml_diff>